<commit_message>
Correción por correción de datos de tensión.
</commit_message>
<xml_diff>
--- a/Datos_tensión.xlsx
+++ b/Datos_tensión.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DARVA\OneDrive\Desktop\Análisis estadístico en R\daaramirezva.tesis.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/daaramirezva_unal_edu_co/Documents/Escritorio/Tesis de maestría/3. Archivos soporte y anexos/4. Tensión y fractura/5. Análisis estadístico en R/daaramirezva.tesis.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150F1A8E-E92F-4912-9670-76878415E60C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{150F1A8E-E92F-4912-9670-76878415E60C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9EC4C49E-4789-4F31-8098-CAF5E687B532}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4EB399ED-FBAD-48C4-B486-975A37C6B8AE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4EB399ED-FBAD-48C4-B486-975A37C6B8AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -108,9 +108,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -433,7 +430,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +451,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>119.84796540304396</v>
+        <v>115.84686971533257</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -462,13 +459,13 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>203.05865706275912</v>
+        <v>199.05705156897849</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -476,13 +473,13 @@
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>208.10627483913703</v>
+        <v>204.50283107021198</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -490,13 +487,13 @@
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>170.4509229178972</v>
+        <v>167.0955755316007</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -504,13 +501,13 @@
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>133.71831311881186</v>
+        <v>129.50778341584157</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -518,13 +515,13 @@
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>149.51085688543247</v>
+        <v>145.50147062310319</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -532,13 +529,13 @@
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>244.41174795122927</v>
+        <v>240.9018738756746</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -546,13 +543,13 @@
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>169.30809978950458</v>
+        <v>166.09720726453887</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -560,13 +557,13 @@
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>142.90452364864865</v>
+        <v>138.88165033783784</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -574,13 +571,13 @@
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>108.49251012145747</v>
+        <v>104.4924812030075</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
@@ -588,13 +585,13 @@
       <c r="C11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>54.352529564019754</v>
+        <v>50.851287637727964</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
@@ -602,13 +599,13 @@
       <c r="C12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>55.296006016042767</v>
+        <v>52.084008546600444</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
@@ -616,13 +613,13 @@
       <c r="C13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>98.716118287225385</v>
+        <v>94.612820382424744</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
@@ -630,13 +627,13 @@
       <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>146.44613011197663</v>
+        <v>142.37455026777019</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>9</v>
@@ -644,13 +641,13 @@
       <c r="C15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>101.1961591135458</v>
+        <v>97.79465886454183</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
@@ -658,13 +655,13 @@
       <c r="C16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>204.37083636495925</v>
+        <v>200.86981410069851</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>9</v>
@@ -672,7 +669,7 @@
       <c r="C17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>